<commit_message>
Validate required values; remove image_type
</commit_message>
<xml_diff>
--- a/spec/fixtures/pop_test_sheet_bad_headers.xlsx
+++ b/spec/fixtures/pop_test_sheet_bad_headers.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="90">
   <si>
     <t>Title Page</t>
   </si>
@@ -160,9 +160,6 @@
     <t>id: place</t>
   </si>
   <si>
-    <t>Provenance</t>
-  </si>
-  <si>
     <t>University of Pennsylvania</t>
   </si>
   <si>
@@ -224,9 +221,6 @@
   </si>
   <si>
     <t>copy: call number/shelf mark</t>
-  </si>
-  <si>
-    <t>evidence: image category</t>
   </si>
   <si>
     <t>evidence: content type</t>
@@ -348,7 +342,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -371,12 +365,6 @@
       <patternFill patternType="solid">
         <fgColor theme="6" tint="0.79998168889431442"/>
         <bgColor rgb="FFD9EAD3"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
@@ -525,7 +513,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -545,7 +533,6 @@
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="79">
@@ -961,13 +948,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AF11"/>
+  <dimension ref="A1:AE11"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="G1" sqref="G1:G1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
@@ -978,42 +965,41 @@
     <col min="4" max="4" width="14.1640625" style="1" customWidth="1"/>
     <col min="5" max="5" width="14.5" style="1"/>
     <col min="6" max="6" width="22.6640625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="17.33203125" style="1" customWidth="1"/>
-    <col min="8" max="8" width="15.1640625" style="1" customWidth="1"/>
-    <col min="9" max="9" width="12.6640625" style="1" customWidth="1"/>
-    <col min="10" max="10" width="20.5" style="1" customWidth="1"/>
-    <col min="11" max="12" width="14.5" style="1" customWidth="1"/>
-    <col min="13" max="13" width="15.5" style="1" customWidth="1"/>
-    <col min="14" max="14" width="13.33203125" style="1" customWidth="1"/>
-    <col min="15" max="15" width="30.1640625" style="1" customWidth="1"/>
-    <col min="16" max="16" width="41.83203125" style="1" customWidth="1"/>
-    <col min="17" max="17" width="34.1640625" style="1" customWidth="1"/>
-    <col min="18" max="18" width="23" style="1" customWidth="1"/>
-    <col min="19" max="19" width="22.1640625" style="1" customWidth="1"/>
-    <col min="20" max="22" width="18.1640625" style="1" customWidth="1"/>
-    <col min="23" max="23" width="8.1640625" style="1" customWidth="1"/>
-    <col min="24" max="24" width="17" style="1" customWidth="1"/>
-    <col min="25" max="25" width="18.1640625" style="1" customWidth="1"/>
-    <col min="26" max="26" width="16.83203125" style="1" customWidth="1"/>
-    <col min="27" max="27" width="18.5" style="1" customWidth="1"/>
-    <col min="28" max="28" width="17.5" style="1" customWidth="1"/>
-    <col min="29" max="29" width="22.6640625" style="1" customWidth="1"/>
-    <col min="30" max="30" width="17.33203125" style="1" customWidth="1"/>
-    <col min="31" max="16384" width="14.5" style="1"/>
+    <col min="7" max="7" width="15.1640625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="12.6640625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="20.5" style="1" customWidth="1"/>
+    <col min="10" max="11" width="14.5" style="1" customWidth="1"/>
+    <col min="12" max="12" width="15.5" style="1" customWidth="1"/>
+    <col min="13" max="13" width="13.33203125" style="1" customWidth="1"/>
+    <col min="14" max="14" width="30.1640625" style="1" customWidth="1"/>
+    <col min="15" max="15" width="41.83203125" style="1" customWidth="1"/>
+    <col min="16" max="16" width="34.1640625" style="1" customWidth="1"/>
+    <col min="17" max="17" width="23" style="1" customWidth="1"/>
+    <col min="18" max="18" width="22.1640625" style="1" customWidth="1"/>
+    <col min="19" max="21" width="18.1640625" style="1" customWidth="1"/>
+    <col min="22" max="22" width="8.1640625" style="1" customWidth="1"/>
+    <col min="23" max="23" width="17" style="1" customWidth="1"/>
+    <col min="24" max="24" width="18.1640625" style="1" customWidth="1"/>
+    <col min="25" max="25" width="16.83203125" style="1" customWidth="1"/>
+    <col min="26" max="26" width="18.5" style="1" customWidth="1"/>
+    <col min="27" max="27" width="17.5" style="1" customWidth="1"/>
+    <col min="28" max="28" width="22.6640625" style="1" customWidth="1"/>
+    <col min="29" max="29" width="17.33203125" style="1" customWidth="1"/>
+    <col min="30" max="16384" width="14.5" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32" ht="15">
+    <row r="1" spans="1:31" ht="15">
       <c r="A1" s="13" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B1" s="13" t="s">
         <v>13</v>
       </c>
       <c r="C1" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="D1" s="14" t="s">
         <v>66</v>
-      </c>
-      <c r="D1" s="14" t="s">
-        <v>67</v>
       </c>
       <c r="E1" s="14" t="s">
         <v>12</v>
@@ -1021,414 +1007,387 @@
       <c r="F1" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="G1" s="16" t="s">
+      <c r="G1" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1" s="15" t="s">
+        <v>67</v>
+      </c>
+      <c r="I1" s="16" t="s">
         <v>68</v>
       </c>
-      <c r="H1" s="15" t="s">
-        <v>10</v>
-      </c>
-      <c r="I1" s="15" t="s">
+      <c r="J1" s="16" t="s">
         <v>69</v>
       </c>
-      <c r="J1" s="17" t="s">
+      <c r="K1" s="16" t="s">
         <v>70</v>
       </c>
-      <c r="K1" s="17" t="s">
+      <c r="L1" s="16" t="s">
         <v>71</v>
       </c>
-      <c r="L1" s="17" t="s">
+      <c r="M1" s="16" t="s">
         <v>72</v>
       </c>
-      <c r="M1" s="17" t="s">
+      <c r="N1" s="16" t="s">
         <v>73</v>
       </c>
-      <c r="N1" s="17" t="s">
+      <c r="O1" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="P1" s="17" t="s">
         <v>74</v>
       </c>
-      <c r="O1" s="17" t="s">
+      <c r="Q1" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="R1" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="S1" s="15" t="s">
         <v>75</v>
       </c>
-      <c r="P1" s="15" t="s">
-        <v>42</v>
-      </c>
-      <c r="Q1" s="18" t="s">
+      <c r="T1" s="15" t="s">
         <v>76</v>
       </c>
-      <c r="R1" s="15" t="s">
-        <v>44</v>
-      </c>
-      <c r="S1" s="15" t="s">
-        <v>41</v>
-      </c>
-      <c r="T1" s="15" t="s">
+      <c r="U1" s="15" t="s">
         <v>77</v>
       </c>
-      <c r="U1" s="15" t="s">
+      <c r="V1" s="18" t="s">
         <v>78</v>
       </c>
-      <c r="V1" s="15" t="s">
+      <c r="W1" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="X1" s="18" t="s">
         <v>79</v>
       </c>
-      <c r="W1" s="19" t="s">
+      <c r="Y1" s="18" t="s">
         <v>80</v>
       </c>
-      <c r="X1" s="19" t="s">
-        <v>45</v>
-      </c>
-      <c r="Y1" s="19" t="s">
+      <c r="Z1" s="18" t="s">
         <v>81</v>
       </c>
-      <c r="Z1" s="19" t="s">
+      <c r="AA1" s="18" t="s">
         <v>82</v>
       </c>
-      <c r="AA1" s="19" t="s">
+      <c r="AB1" s="18" t="s">
         <v>83</v>
       </c>
-      <c r="AB1" s="19" t="s">
+      <c r="AC1" s="18" t="s">
         <v>84</v>
       </c>
-      <c r="AC1" s="19" t="s">
+      <c r="AD1" s="19" t="s">
         <v>85</v>
       </c>
-      <c r="AD1" s="19" t="s">
+      <c r="AE1" s="19" t="s">
         <v>86</v>
       </c>
-      <c r="AE1" s="20" t="s">
+    </row>
+    <row r="2" spans="1:31" ht="15.75" customHeight="1">
+      <c r="A2" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="AF1" s="20" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="2" spans="1:32" ht="15.75" customHeight="1">
-      <c r="A2" s="12" t="s">
-        <v>50</v>
-      </c>
-      <c r="B2" s="11" t="s">
-        <v>52</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>89</v>
-      </c>
       <c r="D2" s="12" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="G2" s="12" t="s">
-        <v>46</v>
-      </c>
-      <c r="H2" s="1" t="s">
+      <c r="G2" s="1" t="s">
         <v>4</v>
       </c>
+      <c r="J2" s="12" t="s">
+        <v>52</v>
+      </c>
       <c r="K2" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="L2" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="M2" s="1">
+        <v>1772</v>
+      </c>
+      <c r="N2" s="12" t="s">
         <v>53</v>
       </c>
-      <c r="L2" s="12" t="s">
+    </row>
+    <row r="3" spans="1:31" ht="15.75" customHeight="1">
+      <c r="A3" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="B3" s="11" t="s">
         <v>51</v>
       </c>
-      <c r="M2" s="12" t="s">
-        <v>61</v>
-      </c>
-      <c r="N2" s="1">
-        <v>1772</v>
-      </c>
-      <c r="O2" s="12" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="3" spans="1:32" ht="15.75" customHeight="1">
-      <c r="A3" s="12" t="s">
-        <v>55</v>
-      </c>
-      <c r="B3" s="11" t="s">
-        <v>52</v>
-      </c>
       <c r="C3" s="1" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D3" s="12" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="G3" s="12" t="s">
-        <v>46</v>
-      </c>
-      <c r="H3" s="1" t="s">
+      <c r="G3" s="1" t="s">
         <v>4</v>
       </c>
+      <c r="J3" s="12" t="s">
+        <v>52</v>
+      </c>
       <c r="K3" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="L3" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="M3" s="1">
+        <v>1772</v>
+      </c>
+      <c r="N3" s="12" t="s">
         <v>53</v>
       </c>
-      <c r="L3" s="12" t="s">
+    </row>
+    <row r="4" spans="1:31" ht="15.75" customHeight="1">
+      <c r="A4" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="B4" s="11" t="s">
         <v>51</v>
       </c>
-      <c r="M3" s="12" t="s">
-        <v>61</v>
-      </c>
-      <c r="N3" s="1">
-        <v>1772</v>
-      </c>
-      <c r="O3" s="12" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="4" spans="1:32" ht="15.75" customHeight="1">
-      <c r="A4" s="12" t="s">
-        <v>56</v>
-      </c>
-      <c r="B4" s="11" t="s">
-        <v>52</v>
-      </c>
       <c r="C4" s="1" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D4" s="12" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="G4" s="12" t="s">
-        <v>46</v>
-      </c>
-      <c r="H4" s="1" t="s">
+      <c r="G4" s="1" t="s">
         <v>4</v>
       </c>
+      <c r="J4" s="12" t="s">
+        <v>52</v>
+      </c>
       <c r="K4" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="L4" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="M4" s="1">
+        <v>1772</v>
+      </c>
+      <c r="N4" s="12" t="s">
         <v>53</v>
       </c>
-      <c r="L4" s="12" t="s">
+    </row>
+    <row r="5" spans="1:31" ht="15.75" customHeight="1">
+      <c r="A5" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="B5" s="11" t="s">
         <v>51</v>
       </c>
-      <c r="M4" s="12" t="s">
-        <v>61</v>
-      </c>
-      <c r="N4" s="1">
-        <v>1772</v>
-      </c>
-      <c r="O4" s="12" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="5" spans="1:32" ht="15.75" customHeight="1">
-      <c r="A5" s="12" t="s">
-        <v>57</v>
-      </c>
-      <c r="B5" s="11" t="s">
-        <v>52</v>
-      </c>
       <c r="C5" s="1" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D5" s="12" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="G5" s="12" t="s">
-        <v>46</v>
+      <c r="J5" s="12" t="s">
+        <v>52</v>
       </c>
       <c r="K5" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="L5" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="M5" s="1">
+        <v>1772</v>
+      </c>
+      <c r="N5" s="12" t="s">
         <v>53</v>
       </c>
-      <c r="L5" s="12" t="s">
+    </row>
+    <row r="6" spans="1:31" ht="15.75" customHeight="1">
+      <c r="A6" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="B6" s="11" t="s">
         <v>51</v>
       </c>
-      <c r="M5" s="12" t="s">
-        <v>61</v>
-      </c>
-      <c r="N5" s="1">
-        <v>1772</v>
-      </c>
-      <c r="O5" s="12" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="6" spans="1:32" ht="15.75" customHeight="1">
-      <c r="A6" s="12" t="s">
-        <v>58</v>
-      </c>
-      <c r="B6" s="11" t="s">
-        <v>52</v>
-      </c>
       <c r="C6" s="1" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D6" s="12" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F6" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G6" s="12" t="s">
+      <c r="G6" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="J6" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="K6" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="L6" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="M6" s="1">
+        <v>1772</v>
+      </c>
+      <c r="N6" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="O6" s="12" t="s">
+        <v>61</v>
+      </c>
+      <c r="X6" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="H6" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="J6" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="K6" s="12" t="s">
-        <v>53</v>
-      </c>
-      <c r="L6" s="12" t="s">
+    </row>
+    <row r="7" spans="1:31" ht="15.75" customHeight="1">
+      <c r="A7" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="B7" s="11" t="s">
         <v>51</v>
       </c>
-      <c r="M6" s="12" t="s">
-        <v>61</v>
-      </c>
-      <c r="N6" s="1">
-        <v>1772</v>
-      </c>
-      <c r="O6" s="12" t="s">
-        <v>54</v>
-      </c>
-      <c r="P6" s="12" t="s">
-        <v>62</v>
-      </c>
-      <c r="Y6" s="1" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="7" spans="1:32" ht="15.75" customHeight="1">
-      <c r="A7" s="12" t="s">
-        <v>59</v>
-      </c>
-      <c r="B7" s="11" t="s">
-        <v>52</v>
-      </c>
       <c r="C7" s="1" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D7" s="12" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F7" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G7" s="12" t="s">
-        <v>46</v>
+      <c r="G7" s="1" t="s">
+        <v>2</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="I7" s="1" t="s">
         <v>37</v>
       </c>
+      <c r="J7" s="12" t="s">
+        <v>52</v>
+      </c>
       <c r="K7" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="L7" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="M7" s="1">
+        <v>1772</v>
+      </c>
+      <c r="N7" s="12" t="s">
         <v>53</v>
       </c>
-      <c r="L7" s="12" t="s">
+      <c r="O7" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="Q7" s="1">
+        <v>1921</v>
+      </c>
+      <c r="V7" s="1">
+        <v>1921</v>
+      </c>
+      <c r="W7" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="8" spans="1:31" ht="15.75" customHeight="1">
+      <c r="A8" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="B8" s="11" t="s">
         <v>51</v>
       </c>
-      <c r="M7" s="12" t="s">
-        <v>61</v>
-      </c>
-      <c r="N7" s="1">
-        <v>1772</v>
-      </c>
-      <c r="O7" s="12" t="s">
-        <v>54</v>
-      </c>
-      <c r="P7" s="12" t="s">
-        <v>63</v>
-      </c>
-      <c r="R7" s="1">
-        <v>1921</v>
-      </c>
-      <c r="W7" s="1">
-        <v>1921</v>
-      </c>
-      <c r="X7" s="1" t="s">
+      <c r="C8" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="D8" s="12" t="s">
         <v>48</v>
-      </c>
-    </row>
-    <row r="8" spans="1:32" ht="15.75" customHeight="1">
-      <c r="A8" s="12" t="s">
-        <v>60</v>
-      </c>
-      <c r="B8" s="11" t="s">
-        <v>52</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="D8" s="12" t="s">
-        <v>49</v>
       </c>
       <c r="F8" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G8" s="12" t="s">
-        <v>46</v>
-      </c>
-      <c r="H8" s="1" t="s">
+      <c r="G8" s="1" t="s">
         <v>28</v>
       </c>
+      <c r="J8" s="12" t="s">
+        <v>52</v>
+      </c>
       <c r="K8" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="L8" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="M8" s="1">
+        <v>1772</v>
+      </c>
+      <c r="N8" s="12" t="s">
         <v>53</v>
       </c>
-      <c r="L8" s="12" t="s">
+      <c r="O8" s="12" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="9" spans="1:31" ht="15.75" customHeight="1">
+      <c r="A9" s="12" t="s">
+        <v>64</v>
+      </c>
+      <c r="B9" s="11" t="s">
         <v>51</v>
       </c>
-      <c r="M8" s="12" t="s">
-        <v>61</v>
-      </c>
-      <c r="N8" s="1">
-        <v>1772</v>
-      </c>
-      <c r="O8" s="12" t="s">
-        <v>54</v>
-      </c>
-      <c r="P8" s="12" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="9" spans="1:32" ht="15.75" customHeight="1">
-      <c r="A9" s="12" t="s">
-        <v>65</v>
-      </c>
-      <c r="B9" s="11" t="s">
-        <v>52</v>
-      </c>
       <c r="C9" s="1" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D9" s="12" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F9" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="G9" s="12" t="s">
-        <v>0</v>
+      <c r="J9" s="12" t="s">
+        <v>52</v>
       </c>
       <c r="K9" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="L9" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="M9" s="1">
+        <v>1772</v>
+      </c>
+      <c r="N9" s="12" t="s">
         <v>53</v>
       </c>
-      <c r="L9" s="12" t="s">
-        <v>51</v>
-      </c>
-      <c r="M9" s="12" t="s">
-        <v>61</v>
-      </c>
-      <c r="N9" s="1">
-        <v>1772</v>
-      </c>
-      <c r="O9" s="12" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="10" spans="1:32" ht="15.75" customHeight="1">
+    </row>
+    <row r="10" spans="1:31" ht="15.75" customHeight="1">
       <c r="A10" s="12"/>
     </row>
-    <row r="11" spans="1:32" ht="15.75" customHeight="1">
+    <row r="11" spans="1:31" ht="15.75" customHeight="1">
       <c r="A11" s="12"/>
     </row>
   </sheetData>
@@ -1460,13 +1419,13 @@
           <x14:formula1>
             <xm:f>'Value lists'!$A$2:$A$12</xm:f>
           </x14:formula1>
-          <xm:sqref>H1:H1048576</xm:sqref>
+          <xm:sqref>G1:G1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>'Value lists'!$C$2:$C$14</xm:f>
           </x14:formula1>
-          <xm:sqref>I1:I1048576</xm:sqref>
+          <xm:sqref>H1:H1048576</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>